<commit_message>
read me file added
</commit_message>
<xml_diff>
--- a/files/output_file_combined.xlsx
+++ b/files/output_file_combined.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>table_header_descriptor</t>
+          <t>table_header_position</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -527,12 +527,20 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>16W</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1600lm</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -564,7 +572,7 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -588,7 +596,7 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -620,7 +628,7 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -644,7 +652,7 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -676,7 +684,7 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -700,7 +708,7 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -740,7 +748,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -759,12 +767,20 @@
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>16W</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1600lm</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -783,20 +799,12 @@
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>16W</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1600lm</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -815,12 +823,20 @@
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>16W</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1600lm</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>"Duxford Range Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the center right position of the page"</t>
+          <t>"Part Number - Can be found on the top right position of the page"</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -860,7 +876,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -884,7 +900,7 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -916,7 +932,7 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -940,7 +956,7 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -972,7 +988,7 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -996,7 +1012,7 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1028,7 +1044,7 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1052,7 +1068,7 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1092,7 +1108,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1116,7 +1132,7 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1148,7 +1164,7 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1172,7 +1188,7 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>"Duxford Range - Can be found on the right side of the page"</t>
+          <t>"Part Number Description Dimensions Power Lumens Colour Temp. - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H25" t="n">

</xml_diff>